<commit_message>
Fixup: Use CEA instead of EPSG:3857
</commit_message>
<xml_diff>
--- a/deepstate.xlsx
+++ b/deepstate.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C531"/>
+  <dimension ref="A1:C547"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>138166.94064694</v>
+        <v>62920.84966366</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>138166.94064694</v>
+        <v>62920.84966366</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>138799.66503575</v>
+        <v>63214.57991599</v>
       </c>
     </row>
     <row r="5">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>138799.66503575</v>
+        <v>63214.57991599</v>
       </c>
     </row>
     <row r="6">
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>142289.31130201</v>
+        <v>64689.18705694001</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>142289.31130201</v>
+        <v>64689.18705694001</v>
       </c>
     </row>
     <row r="8">
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>142584.16924431</v>
+        <v>64806.21963948999</v>
       </c>
     </row>
     <row r="9">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>140217.95557983</v>
+        <v>63867.56917078</v>
       </c>
     </row>
     <row r="10">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>140552.68079639</v>
+        <v>64016.97279823</v>
       </c>
     </row>
     <row r="11">
@@ -583,7 +583,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>140446.75259456</v>
+        <v>63966.75848065</v>
       </c>
     </row>
     <row r="12">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>140522.94398054</v>
+        <v>63998.73993046</v>
       </c>
     </row>
     <row r="13">
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>140976.96597552</v>
+        <v>64186.56592389</v>
       </c>
     </row>
     <row r="14">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>140622.57765173</v>
+        <v>64026.05337905</v>
       </c>
     </row>
     <row r="15">
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>140622.57765173</v>
+        <v>64026.05337905</v>
       </c>
     </row>
     <row r="16">
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>140540.66659426</v>
+        <v>63988.57673784999</v>
       </c>
     </row>
     <row r="17">
@@ -661,7 +661,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>140540.66659426</v>
+        <v>63988.57673784999</v>
       </c>
     </row>
     <row r="18">
@@ -674,7 +674,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>140790.21111539</v>
+        <v>64100.44749233</v>
       </c>
     </row>
     <row r="19">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>143872.93659735</v>
+        <v>65375.29071184</v>
       </c>
     </row>
     <row r="20">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>143872.93659735</v>
+        <v>65375.29071184</v>
       </c>
     </row>
     <row r="21">
@@ -713,7 +713,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>143872.93659735</v>
+        <v>65375.29071184</v>
       </c>
     </row>
     <row r="22">
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>146115.77918692</v>
+        <v>66319.31041706</v>
       </c>
     </row>
     <row r="23">
@@ -739,7 +739,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>146115.77918692</v>
+        <v>66319.31041706</v>
       </c>
     </row>
     <row r="24">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>146122.85840427</v>
+        <v>66322.59855182</v>
       </c>
     </row>
     <row r="25">
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>145688.52200171</v>
+        <v>66119.08831507</v>
       </c>
     </row>
     <row r="26">
@@ -778,7 +778,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>145680.4882247</v>
+        <v>66115.4281053</v>
       </c>
     </row>
     <row r="27">
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>145680.4882247</v>
+        <v>66115.4281053</v>
       </c>
     </row>
     <row r="28">
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>145680.4882247</v>
+        <v>66115.4281053</v>
       </c>
     </row>
     <row r="29">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>145752.66638374</v>
+        <v>66149.19168074</v>
       </c>
     </row>
     <row r="30">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>145752.66638374</v>
+        <v>66149.19168074</v>
       </c>
     </row>
     <row r="31">
@@ -843,7 +843,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>145752.66638374</v>
+        <v>66149.19168074</v>
       </c>
     </row>
     <row r="32">
@@ -856,7 +856,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>146219.6955745</v>
+        <v>66371.47592934</v>
       </c>
     </row>
     <row r="33">
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>146194.61900515</v>
+        <v>66360.6918424</v>
       </c>
     </row>
     <row r="34">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>151691.76303304</v>
+        <v>68679.31219378</v>
       </c>
     </row>
     <row r="35">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>151537.88911313</v>
+        <v>68609.33207737</v>
       </c>
     </row>
     <row r="36">
@@ -908,7 +908,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>156930.89920318</v>
+        <v>71107.76774789</v>
       </c>
     </row>
     <row r="37">
@@ -921,7 +921,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>157478.37296793</v>
+        <v>71349.56804622</v>
       </c>
     </row>
     <row r="38">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>157486.91901444</v>
+        <v>71353.5277475</v>
       </c>
     </row>
     <row r="39">
@@ -947,7 +947,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>157486.91901444</v>
+        <v>71353.5277475</v>
       </c>
     </row>
     <row r="40">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>157721.24116467</v>
+        <v>71453.10991888</v>
       </c>
     </row>
     <row r="41">
@@ -973,7 +973,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>157721.29530658</v>
+        <v>71453.15958974001</v>
       </c>
     </row>
     <row r="42">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>157736.67184682</v>
+        <v>71457.01578338</v>
       </c>
     </row>
     <row r="43">
@@ -999,7 +999,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>157684.13526057</v>
+        <v>71434.43294831</v>
       </c>
     </row>
     <row r="44">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>157683.3237987</v>
+        <v>71433.73003696001</v>
       </c>
     </row>
     <row r="45">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>159247.4245329</v>
+        <v>72091.04945063</v>
       </c>
     </row>
     <row r="46">
@@ -1038,7 +1038,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>159263.44101595</v>
+        <v>72098.48507025</v>
       </c>
     </row>
     <row r="47">
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>159263.44101595</v>
+        <v>72098.48507025</v>
       </c>
     </row>
     <row r="48">
@@ -1064,7 +1064,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>159297.11524418</v>
+        <v>72113.36945457001</v>
       </c>
     </row>
     <row r="49">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>159347.28231488</v>
+        <v>72135.8306133</v>
       </c>
     </row>
     <row r="50">
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>159373.70216884</v>
+        <v>72147.95434294999</v>
       </c>
     </row>
     <row r="51">
@@ -1103,7 +1103,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>159386.2000146</v>
+        <v>72153.32898214999</v>
       </c>
     </row>
     <row r="52">
@@ -1116,7 +1116,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>164198.6185985</v>
+        <v>74173.75318869999</v>
       </c>
     </row>
     <row r="53">
@@ -1129,7 +1129,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>164678.00363245</v>
+        <v>74390.90374638001</v>
       </c>
     </row>
     <row r="54">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>164807.65319286</v>
+        <v>74446.39482011</v>
       </c>
     </row>
     <row r="55">
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>169340.18979992</v>
+        <v>76337.13687613999</v>
       </c>
     </row>
     <row r="56">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>169146.52715692</v>
+        <v>76244.34752007</v>
       </c>
     </row>
     <row r="57">
@@ -1181,7 +1181,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>169189.65262936</v>
+        <v>76263.43689525999</v>
       </c>
     </row>
     <row r="58">
@@ -1194,7 +1194,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>169307.90975579</v>
+        <v>76314.72824959</v>
       </c>
     </row>
     <row r="59">
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>169307.90975579</v>
+        <v>76314.72824959</v>
       </c>
     </row>
     <row r="60">
@@ -1220,7 +1220,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>169755.42097726</v>
+        <v>76520.42126783</v>
       </c>
     </row>
     <row r="61">
@@ -1233,7 +1233,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>170517.87259526</v>
+        <v>76845.15176653999</v>
       </c>
     </row>
     <row r="62">
@@ -1246,7 +1246,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>170694.77937421</v>
+        <v>76920.69111711001</v>
       </c>
     </row>
     <row r="63">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>171117.61073909</v>
+        <v>77118.12046655999</v>
       </c>
     </row>
     <row r="64">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>171117.62993854</v>
+        <v>77118.12928582</v>
       </c>
     </row>
     <row r="65">
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>171219.60617822</v>
+        <v>77161.94100288</v>
       </c>
     </row>
     <row r="66">
@@ -1298,7 +1298,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>172777.2763222</v>
+        <v>77825.3239321</v>
       </c>
     </row>
     <row r="67">
@@ -1311,7 +1311,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>172922.91590378</v>
+        <v>77893.35480553999</v>
       </c>
     </row>
     <row r="68">
@@ -1324,7 +1324,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>172903.65314493</v>
+        <v>77885.4008187</v>
       </c>
     </row>
     <row r="69">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>172883.24668629</v>
+        <v>77873.11221466999</v>
       </c>
     </row>
     <row r="70">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>172822.4265391</v>
+        <v>77846.4635974</v>
       </c>
     </row>
     <row r="71">
@@ -1363,7 +1363,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>172814.23984428</v>
+        <v>77843.08569771</v>
       </c>
     </row>
     <row r="72">
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>172814.23984428</v>
+        <v>77843.08569771</v>
       </c>
     </row>
     <row r="73">
@@ -1389,7 +1389,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>172814.2603419</v>
+        <v>77843.09410647</v>
       </c>
     </row>
     <row r="74">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>172940.81413229</v>
+        <v>77897.24196855001</v>
       </c>
     </row>
     <row r="75">
@@ -1415,7 +1415,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>172940.81413229</v>
+        <v>77897.24196855001</v>
       </c>
     </row>
     <row r="76">
@@ -1428,7 +1428,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>172996.74376021</v>
+        <v>77921.6790111</v>
       </c>
     </row>
     <row r="77">
@@ -1441,7 +1441,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>173028.84144581</v>
+        <v>77935.53979914999</v>
       </c>
     </row>
     <row r="78">
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>173018.20903606</v>
+        <v>77925.28120869001</v>
       </c>
     </row>
     <row r="79">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>173018.20903606</v>
+        <v>77925.28120869001</v>
       </c>
     </row>
     <row r="80">
@@ -1480,7 +1480,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>173070.73159281</v>
+        <v>77948.6180761</v>
       </c>
     </row>
     <row r="81">
@@ -1493,7 +1493,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>172986.0562858</v>
+        <v>77914.18755932001</v>
       </c>
     </row>
     <row r="82">
@@ -1506,7 +1506,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>172986.0562858</v>
+        <v>77914.18755932001</v>
       </c>
     </row>
     <row r="83">
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>174077.8314688</v>
+        <v>78416.32795834</v>
       </c>
     </row>
     <row r="84">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>174077.8314688</v>
+        <v>78416.32795834</v>
       </c>
     </row>
     <row r="85">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>174289.66895187</v>
+        <v>78508.30801137</v>
       </c>
     </row>
     <row r="86">
@@ -1558,7 +1558,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>174274.01445202</v>
+        <v>78501.59139307</v>
       </c>
     </row>
     <row r="87">
@@ -1571,7 +1571,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>174375.69139858</v>
+        <v>78545.54305764</v>
       </c>
     </row>
     <row r="88">
@@ -1584,7 +1584,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>174372.72316021</v>
+        <v>78544.45295228</v>
       </c>
     </row>
     <row r="89">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>174266.95189488</v>
+        <v>78503.09296289999</v>
       </c>
     </row>
     <row r="90">
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>174141.31955464</v>
+        <v>78451.49910236</v>
       </c>
     </row>
     <row r="91">
@@ -1623,7 +1623,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>174184.54903156</v>
+        <v>78470.03204619999</v>
       </c>
     </row>
     <row r="92">
@@ -1636,7 +1636,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>174184.54903156</v>
+        <v>78470.03204619999</v>
       </c>
     </row>
     <row r="93">
@@ -1649,7 +1649,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>173732.16283976</v>
+        <v>78283.1714218</v>
       </c>
     </row>
     <row r="94">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>173732.16283976</v>
+        <v>78283.1714218</v>
       </c>
     </row>
     <row r="95">
@@ -1675,7 +1675,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>173835.82869948</v>
+        <v>78328.54758742999</v>
       </c>
     </row>
     <row r="96">
@@ -1688,7 +1688,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>174099.54565984</v>
+        <v>78442.25517402</v>
       </c>
     </row>
     <row r="97">
@@ -1701,7 +1701,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>173574.63210309</v>
+        <v>78205.99407938001</v>
       </c>
     </row>
     <row r="98">
@@ -1714,7 +1714,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>173574.63210309</v>
+        <v>78205.99407938001</v>
       </c>
     </row>
     <row r="99">
@@ -1727,7 +1727,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>173872.96562061</v>
+        <v>78341.99207405999</v>
       </c>
     </row>
     <row r="100">
@@ -1740,7 +1740,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>173872.96562061</v>
+        <v>78341.99207405999</v>
       </c>
     </row>
     <row r="101">
@@ -1753,7 +1753,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>173872.96562061</v>
+        <v>78341.99207405999</v>
       </c>
     </row>
     <row r="102">
@@ -1766,7 +1766,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>173859.74459014</v>
+        <v>78336.57724717999</v>
       </c>
     </row>
     <row r="103">
@@ -1779,7 +1779,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>173818.27522111</v>
+        <v>78319.55157428001</v>
       </c>
     </row>
     <row r="104">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>174288.8354859</v>
+        <v>78537.95088785001</v>
       </c>
     </row>
     <row r="105">
@@ -1805,7 +1805,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>265757.54847685</v>
+        <v>121961.28043705</v>
       </c>
     </row>
     <row r="106">
@@ -1818,7 +1818,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>265760.59748735</v>
+        <v>121962.53472412</v>
       </c>
     </row>
     <row r="107">
@@ -1831,7 +1831,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>265648.7265479</v>
+        <v>121910.19427115</v>
       </c>
     </row>
     <row r="108">
@@ -1844,7 +1844,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>265683.66393187</v>
+        <v>121924.94178551</v>
       </c>
     </row>
     <row r="109">
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>265764.286737</v>
+        <v>121960.87149603</v>
       </c>
     </row>
     <row r="110">
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>265756.90998887</v>
+        <v>121957.69733438</v>
       </c>
     </row>
     <row r="111">
@@ -1883,7 +1883,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>265700.47571945</v>
+        <v>121944.38149854</v>
       </c>
     </row>
     <row r="112">
@@ -1896,7 +1896,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>266224.18110074</v>
+        <v>122169.27459826</v>
       </c>
     </row>
     <row r="113">
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>265788.78990649</v>
+        <v>121966.41465257</v>
       </c>
     </row>
     <row r="114">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>265478.30825763</v>
+        <v>121838.60936998</v>
       </c>
     </row>
     <row r="115">
@@ -1935,7 +1935,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>265651.59966937</v>
+        <v>121914.95144998</v>
       </c>
     </row>
     <row r="116">
@@ -1948,7 +1948,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>265684.18109101</v>
+        <v>121928.39066953</v>
       </c>
     </row>
     <row r="117">
@@ -1961,7 +1961,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>264972.68176774</v>
+        <v>121608.98426339</v>
       </c>
     </row>
     <row r="118">
@@ -1974,7 +1974,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>265147.74015325</v>
+        <v>121687.61347036</v>
       </c>
     </row>
     <row r="119">
@@ -1987,7 +1987,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>266167.14288295</v>
+        <v>122140.77398903</v>
       </c>
     </row>
     <row r="120">
@@ -2000,7 +2000,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>266334.31786326</v>
+        <v>122213.2931441</v>
       </c>
     </row>
     <row r="121">
@@ -2013,7 +2013,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>266345.96467638</v>
+        <v>122218.93458745</v>
       </c>
     </row>
     <row r="122">
@@ -2026,7 +2026,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>266454.16097553</v>
+        <v>122266.14409314</v>
       </c>
     </row>
     <row r="123">
@@ -2039,7 +2039,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>266654.48520849</v>
+        <v>122350.14599157</v>
       </c>
     </row>
     <row r="124">
@@ -2052,7 +2052,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>266578.60542593</v>
+        <v>122319.50659697</v>
       </c>
     </row>
     <row r="125">
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>266613.97970677</v>
+        <v>122335.06548313</v>
       </c>
     </row>
     <row r="126">
@@ -2078,7 +2078,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>266673.79980451</v>
+        <v>122360.94520154</v>
       </c>
     </row>
     <row r="127">
@@ -2091,7 +2091,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>266746.41494698</v>
+        <v>122392.72664975</v>
       </c>
     </row>
     <row r="128">
@@ -2104,7 +2104,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>267076.39630161</v>
+        <v>122537.94315933</v>
       </c>
     </row>
     <row r="129">
@@ -2117,7 +2117,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>267076.39630161</v>
+        <v>122537.94315933</v>
       </c>
     </row>
     <row r="130">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>267198.27458489</v>
+        <v>122589.51838731</v>
       </c>
     </row>
     <row r="131">
@@ -2143,7 +2143,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>267177.54383358</v>
+        <v>122580.45674935</v>
       </c>
     </row>
     <row r="132">
@@ -2156,7 +2156,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>267207.31423468</v>
+        <v>122593.29088971</v>
       </c>
     </row>
     <row r="133">
@@ -2169,7 +2169,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>267192.82986358</v>
+        <v>122586.9764597</v>
       </c>
     </row>
     <row r="134">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>267345.32899598</v>
+        <v>122653.70295204</v>
       </c>
     </row>
     <row r="135">
@@ -2195,7 +2195,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>267411.17689322</v>
+        <v>122682.11896024</v>
       </c>
     </row>
     <row r="136">
@@ -2208,7 +2208,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>267496.9335854</v>
+        <v>122718.91273881</v>
       </c>
     </row>
     <row r="137">
@@ -2221,7 +2221,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>267322.54885475</v>
+        <v>122640.75153496</v>
       </c>
     </row>
     <row r="138">
@@ -2234,7 +2234,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>267444.00668663</v>
+        <v>122693.01505771</v>
       </c>
     </row>
     <row r="139">
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>267460.88913775</v>
+        <v>122700.16051611</v>
       </c>
     </row>
     <row r="140">
@@ -2260,7 +2260,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>267408.2477308</v>
+        <v>122675.52304192</v>
       </c>
     </row>
     <row r="141">
@@ -2273,7 +2273,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>267384.85388772</v>
+        <v>122664.92340096</v>
       </c>
     </row>
     <row r="142">
@@ -2286,7 +2286,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>267322.58029115</v>
+        <v>122637.77320595</v>
       </c>
     </row>
     <row r="143">
@@ -2299,7 +2299,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>267281.7298418</v>
+        <v>122614.17041656</v>
       </c>
     </row>
     <row r="144">
@@ -2312,7 +2312,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>267190.03005601</v>
+        <v>122572.69729503</v>
       </c>
     </row>
     <row r="145">
@@ -2325,7 +2325,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>267237.87094847</v>
+        <v>122592.79101958</v>
       </c>
     </row>
     <row r="146">
@@ -2338,7 +2338,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>267441.14864048</v>
+        <v>122685.94186011</v>
       </c>
     </row>
     <row r="147">
@@ -2351,7 +2351,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>267494.61405151</v>
+        <v>122710.03042586</v>
       </c>
     </row>
     <row r="148">
@@ -2364,7 +2364,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>267494.61405151</v>
+        <v>122710.03042586</v>
       </c>
     </row>
     <row r="149">
@@ -2377,7 +2377,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>267494.61405151</v>
+        <v>122710.03042586</v>
       </c>
     </row>
     <row r="150">
@@ -2390,7 +2390,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>267501.00269829</v>
+        <v>122712.77874165</v>
       </c>
     </row>
     <row r="151">
@@ -2403,7 +2403,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>267544.90802581</v>
+        <v>122731.4900746</v>
       </c>
     </row>
     <row r="152">
@@ -2416,7 +2416,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>267544.90802581</v>
+        <v>122731.4900746</v>
       </c>
     </row>
     <row r="153">
@@ -2429,7 +2429,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>267583.09415781</v>
+        <v>122748.96138702</v>
       </c>
     </row>
     <row r="154">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>267614.92395268</v>
+        <v>122762.63925898</v>
       </c>
     </row>
     <row r="155">
@@ -2455,7 +2455,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>267686.58938706</v>
+        <v>122792.10227425</v>
       </c>
     </row>
     <row r="156">
@@ -2468,7 +2468,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>267538.90074571</v>
+        <v>122724.40224028</v>
       </c>
     </row>
     <row r="157">
@@ -2481,7 +2481,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>268007.80203105</v>
+        <v>122925.44402368</v>
       </c>
     </row>
     <row r="158">
@@ -2494,7 +2494,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>267993.84443079</v>
+        <v>122919.4137614</v>
       </c>
     </row>
     <row r="159">
@@ -2507,7 +2507,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>268074.31919947</v>
+        <v>122952.60867228</v>
       </c>
     </row>
     <row r="160">
@@ -2520,7 +2520,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>268074.31919947</v>
+        <v>122952.60867228</v>
       </c>
     </row>
     <row r="161">
@@ -2533,7 +2533,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>268221.70491214</v>
+        <v>123016.02977168</v>
       </c>
     </row>
     <row r="162">
@@ -2546,7 +2546,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>268264.70226516</v>
+        <v>123036.27960343</v>
       </c>
     </row>
     <row r="163">
@@ -2559,7 +2559,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>268071.55241355</v>
+        <v>122957.22590582</v>
       </c>
     </row>
     <row r="164">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>268191.67219511</v>
+        <v>123008.80724765</v>
       </c>
     </row>
     <row r="165">
@@ -2585,7 +2585,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>268255.38196413</v>
+        <v>123036.17246982</v>
       </c>
     </row>
     <row r="166">
@@ -2598,7 +2598,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>268255.38196413</v>
+        <v>123036.17246982</v>
       </c>
     </row>
     <row r="167">
@@ -2611,7 +2611,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>268275.25531317</v>
+        <v>123044.70973996</v>
       </c>
     </row>
     <row r="168">
@@ -2624,7 +2624,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>268481.56578658</v>
+        <v>123129.98212332</v>
       </c>
     </row>
     <row r="169">
@@ -2637,7 +2637,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>268481.56578658</v>
+        <v>123129.98212332</v>
       </c>
     </row>
     <row r="170">
@@ -2650,7 +2650,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>268468.47829193</v>
+        <v>123124.62277556</v>
       </c>
     </row>
     <row r="171">
@@ -2663,7 +2663,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>268555.80816184</v>
+        <v>123164.26319526</v>
       </c>
     </row>
     <row r="172">
@@ -2676,7 +2676,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>268575.78401363</v>
+        <v>123172.85780978</v>
       </c>
     </row>
     <row r="173">
@@ -2689,7 +2689,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>268575.78401363</v>
+        <v>123172.85780978</v>
       </c>
     </row>
     <row r="174">
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>268575.78401363</v>
+        <v>123172.85780978</v>
       </c>
     </row>
     <row r="175">
@@ -2715,7 +2715,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>268996.85117863</v>
+        <v>123352.16094778</v>
       </c>
     </row>
     <row r="176">
@@ -2728,7 +2728,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>269359.1986727</v>
+        <v>123501.95094421</v>
       </c>
     </row>
     <row r="177">
@@ -2741,7 +2741,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>269541.91693194</v>
+        <v>123582.3810958</v>
       </c>
     </row>
     <row r="178">
@@ -2754,7 +2754,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>269578.83826989</v>
+        <v>123598.58884438</v>
       </c>
     </row>
     <row r="179">
@@ -2767,7 +2767,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>269910.14691854</v>
+        <v>123738.96260997</v>
       </c>
     </row>
     <row r="180">
@@ -2780,7 +2780,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>269947.69869325</v>
+        <v>123755.14919889</v>
       </c>
     </row>
     <row r="181">
@@ -2793,7 +2793,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>270015.20203934</v>
+        <v>123784.34384082</v>
       </c>
     </row>
     <row r="182">
@@ -2806,7 +2806,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>270015.20203934</v>
+        <v>123784.34384082</v>
       </c>
     </row>
     <row r="183">
@@ -2819,7 +2819,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>270066.39818684</v>
+        <v>123808.50279039</v>
       </c>
     </row>
     <row r="184">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>270077.26815962</v>
+        <v>123814.34853426</v>
       </c>
     </row>
     <row r="185">
@@ -2845,7 +2845,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>270275.18712151</v>
+        <v>123903.68146181</v>
       </c>
     </row>
     <row r="186">
@@ -2858,7 +2858,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>270351.94099364</v>
+        <v>123938.2156508</v>
       </c>
     </row>
     <row r="187">
@@ -2871,7 +2871,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>270377.86964502</v>
+        <v>123949.60760476</v>
       </c>
     </row>
     <row r="188">
@@ -2884,7 +2884,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>270380.10384693</v>
+        <v>123950.94455655</v>
       </c>
     </row>
     <row r="189">
@@ -2897,7 +2897,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>270412.83473095</v>
+        <v>123965.1650036</v>
       </c>
     </row>
     <row r="190">
@@ -2910,7 +2910,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>270416.19261425</v>
+        <v>123966.62363682</v>
       </c>
     </row>
     <row r="191">
@@ -2923,7 +2923,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>270449.57044432</v>
+        <v>123981.11704026</v>
       </c>
     </row>
     <row r="192">
@@ -2936,7 +2936,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>270231.50022361</v>
+        <v>123879.86163471</v>
       </c>
     </row>
     <row r="193">
@@ -2949,7 +2949,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>270265.03088776</v>
+        <v>123894.45074888</v>
       </c>
     </row>
     <row r="194">
@@ -2962,7 +2962,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>270360.00684094</v>
+        <v>123939.01545252</v>
       </c>
     </row>
     <row r="195">
@@ -2975,7 +2975,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>270506.78560476</v>
+        <v>124001.71922285</v>
       </c>
     </row>
     <row r="196">
@@ -2988,7 +2988,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>270541.36586944</v>
+        <v>124016.9747788</v>
       </c>
     </row>
     <row r="197">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>270554.46918032</v>
+        <v>124022.67117416</v>
       </c>
     </row>
     <row r="198">
@@ -3014,7 +3014,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>270540.57926271</v>
+        <v>124016.85942214</v>
       </c>
     </row>
     <row r="199">
@@ -3027,7 +3027,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>270585.95140303</v>
+        <v>124036.38405172</v>
       </c>
     </row>
     <row r="200">
@@ -3040,7 +3040,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>270587.3802204</v>
+        <v>124037.03574398</v>
       </c>
     </row>
     <row r="201">
@@ -3053,7 +3053,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>270792.9328214</v>
+        <v>124122.63648624</v>
       </c>
     </row>
     <row r="202">
@@ -3066,7 +3066,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>270877.68771817</v>
+        <v>124157.77351202</v>
       </c>
     </row>
     <row r="203">
@@ -3079,7 +3079,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>270903.33150758</v>
+        <v>124168.89775803</v>
       </c>
     </row>
     <row r="204">
@@ -3092,7 +3092,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>270962.26543209</v>
+        <v>124194.45745338</v>
       </c>
     </row>
     <row r="205">
@@ -3105,7 +3105,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>270964.42413015</v>
+        <v>124193.51472874</v>
       </c>
     </row>
     <row r="206">
@@ -3118,7 +3118,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>271102.78648242</v>
+        <v>124252.08248889</v>
       </c>
     </row>
     <row r="207">
@@ -3131,7 +3131,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>271071.00527446</v>
+        <v>124239.08045675</v>
       </c>
     </row>
     <row r="208">
@@ -3144,7 +3144,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>271234.11466037</v>
+        <v>124309.64235124</v>
       </c>
     </row>
     <row r="209">
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>271255.60816526</v>
+        <v>124318.95207719</v>
       </c>
     </row>
     <row r="210">
@@ -3170,7 +3170,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>271272.0769728</v>
+        <v>124326.09081902</v>
       </c>
     </row>
     <row r="211">
@@ -3183,7 +3183,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>271338.29598941</v>
+        <v>124354.62187015</v>
       </c>
     </row>
     <row r="212">
@@ -3196,7 +3196,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>271316.78412831</v>
+        <v>124344.80646756</v>
       </c>
     </row>
     <row r="213">
@@ -3209,7 +3209,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>271522.83751294</v>
+        <v>124434.07555947</v>
       </c>
     </row>
     <row r="214">
@@ -3222,7 +3222,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>271522.83751294</v>
+        <v>124434.07555947</v>
       </c>
     </row>
     <row r="215">
@@ -3235,7 +3235,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>271522.83751294</v>
+        <v>124434.07555947</v>
       </c>
     </row>
     <row r="216">
@@ -3248,7 +3248,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>271820.87802165</v>
+        <v>124562.99545036</v>
       </c>
     </row>
     <row r="217">
@@ -3261,7 +3261,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>271820.22691643</v>
+        <v>124563.01289762</v>
       </c>
     </row>
     <row r="218">
@@ -3274,7 +3274,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>271820.22691643</v>
+        <v>124563.01289762</v>
       </c>
     </row>
     <row r="219">
@@ -3287,7 +3287,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>272421.89715053</v>
+        <v>124820.11622199</v>
       </c>
     </row>
     <row r="220">
@@ -3300,7 +3300,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>272490.49422996</v>
+        <v>124849.89603684</v>
       </c>
     </row>
     <row r="221">
@@ -3313,7 +3313,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>272508.41983586</v>
+        <v>124857.62131918</v>
       </c>
     </row>
     <row r="222">
@@ -3326,7 +3326,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>272509.55073362</v>
+        <v>124858.09719745</v>
       </c>
     </row>
     <row r="223">
@@ -3339,7 +3339,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>272525.10379885</v>
+        <v>124864.92346169</v>
       </c>
     </row>
     <row r="224">
@@ -3352,7 +3352,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>272563.33415836</v>
+        <v>124881.77128389</v>
       </c>
     </row>
     <row r="225">
@@ -3365,7 +3365,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>272536.06421411</v>
+        <v>124869.62395964</v>
       </c>
     </row>
     <row r="226">
@@ -3378,7 +3378,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>272674.46948581</v>
+        <v>124931.0273543</v>
       </c>
     </row>
     <row r="227">
@@ -3391,7 +3391,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>272669.8620882</v>
+        <v>124929.00479073</v>
       </c>
     </row>
     <row r="228">
@@ -3404,7 +3404,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>272650.7844762</v>
+        <v>124920.7855369</v>
       </c>
     </row>
     <row r="229">
@@ -3417,7 +3417,7 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>272681.46379775</v>
+        <v>124934.04758649</v>
       </c>
     </row>
     <row r="230">
@@ -3430,7 +3430,7 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>272675.33138005</v>
+        <v>124931.76264068</v>
       </c>
     </row>
     <row r="231">
@@ -3443,7 +3443,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>272589.01267664</v>
+        <v>124896.51730971</v>
       </c>
     </row>
     <row r="232">
@@ -3456,7 +3456,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>272602.5547037</v>
+        <v>124902.39601054</v>
       </c>
     </row>
     <row r="233">
@@ -3469,7 +3469,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>272628.77117894</v>
+        <v>124913.791162</v>
       </c>
     </row>
     <row r="234">
@@ -3482,7 +3482,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>272575.32134835</v>
+        <v>124890.38969698</v>
       </c>
     </row>
     <row r="235">
@@ -3495,7 +3495,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>272341.89508106</v>
+        <v>124783.89114681</v>
       </c>
     </row>
     <row r="236">
@@ -3508,7 +3508,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>272426.75770737</v>
+        <v>124822.0850154</v>
       </c>
     </row>
     <row r="237">
@@ -3521,7 +3521,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>272426.75770737</v>
+        <v>124822.0850154</v>
       </c>
     </row>
     <row r="238">
@@ -3534,7 +3534,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>272437.8304192</v>
+        <v>124827.00960901</v>
       </c>
     </row>
     <row r="239">
@@ -3547,7 +3547,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>272406.38619862</v>
+        <v>124813.55735009</v>
       </c>
     </row>
     <row r="240">
@@ -3560,7 +3560,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>272415.60149272</v>
+        <v>124817.69706978</v>
       </c>
     </row>
     <row r="241">
@@ -3573,7 +3573,7 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>272340.68821286</v>
+        <v>124783.34865494</v>
       </c>
     </row>
     <row r="242">
@@ -3586,7 +3586,7 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>272354.86740321</v>
+        <v>124789.04553201</v>
       </c>
     </row>
     <row r="243">
@@ -3599,7 +3599,7 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>272447.51633487</v>
+        <v>124832.59073303</v>
       </c>
     </row>
     <row r="244">
@@ -3612,7 +3612,7 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>272444.05515645</v>
+        <v>124830.98823461</v>
       </c>
     </row>
     <row r="245">
@@ -3625,7 +3625,7 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>272444.05515645</v>
+        <v>124830.98823461</v>
       </c>
     </row>
     <row r="246">
@@ -3638,7 +3638,7 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>272384.53923113</v>
+        <v>124805.34252807</v>
       </c>
     </row>
     <row r="247">
@@ -3651,7 +3651,7 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>272428.75313271</v>
+        <v>124824.58399574</v>
       </c>
     </row>
     <row r="248">
@@ -3664,7 +3664,7 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>272453.34940187</v>
+        <v>124835.41067046</v>
       </c>
     </row>
     <row r="249">
@@ -3677,7 +3677,7 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>272503.3076529</v>
+        <v>124856.79831218</v>
       </c>
     </row>
     <row r="250">
@@ -3690,7 +3690,7 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>272503.3076529</v>
+        <v>124856.79831218</v>
       </c>
     </row>
     <row r="251">
@@ -3703,7 +3703,7 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>272503.3076529</v>
+        <v>124856.79831218</v>
       </c>
     </row>
     <row r="252">
@@ -3716,7 +3716,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>272475.08517101</v>
+        <v>124844.86161089</v>
       </c>
     </row>
     <row r="253">
@@ -3729,7 +3729,7 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>272465.35417511</v>
+        <v>124840.94153193</v>
       </c>
     </row>
     <row r="254">
@@ -3742,7 +3742,7 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>272452.90050579</v>
+        <v>124835.24467512</v>
       </c>
     </row>
     <row r="255">
@@ -3755,7 +3755,7 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>272428.18794562</v>
+        <v>124824.26613292</v>
       </c>
     </row>
     <row r="256">
@@ -3768,7 +3768,7 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>272462.92268424</v>
+        <v>124839.45124586</v>
       </c>
     </row>
     <row r="257">
@@ -3781,7 +3781,7 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>272508.79347737</v>
+        <v>124859.90285494</v>
       </c>
     </row>
     <row r="258">
@@ -3794,7 +3794,7 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>272597.44320823</v>
+        <v>124898.89923253</v>
       </c>
     </row>
     <row r="259">
@@ -3807,7 +3807,7 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>272485.49957001</v>
+        <v>124850.8309061</v>
       </c>
     </row>
     <row r="260">
@@ -3820,7 +3820,7 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>272444.90073391</v>
+        <v>124833.68277911</v>
       </c>
     </row>
     <row r="261">
@@ -3833,7 +3833,7 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>272407.99696038</v>
+        <v>124817.81016734</v>
       </c>
     </row>
     <row r="262">
@@ -3846,7 +3846,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>272396.52707881</v>
+        <v>124812.70856239</v>
       </c>
     </row>
     <row r="263">
@@ -3859,7 +3859,7 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>272438.29596689</v>
+        <v>124831.44319969</v>
       </c>
     </row>
     <row r="264">
@@ -3872,7 +3872,7 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>272450.57870824</v>
+        <v>124836.48422576</v>
       </c>
     </row>
     <row r="265">
@@ -3885,7 +3885,7 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>272519.95789223</v>
+        <v>124866.45734432</v>
       </c>
     </row>
     <row r="266">
@@ -3898,7 +3898,7 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>272558.78750398</v>
+        <v>124883.8890357</v>
       </c>
     </row>
     <row r="267">
@@ -3911,7 +3911,7 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>272569.4911694</v>
+        <v>124888.42944423</v>
       </c>
     </row>
     <row r="268">
@@ -3924,7 +3924,7 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>272569.4911694</v>
+        <v>124888.42944423</v>
       </c>
     </row>
     <row r="269">
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>272634.20836992</v>
+        <v>124917.05770224</v>
       </c>
     </row>
     <row r="270">
@@ -3950,7 +3950,7 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>272638.63942092</v>
+        <v>124919.03798794</v>
       </c>
     </row>
     <row r="271">
@@ -3963,7 +3963,7 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>272657.33138657</v>
+        <v>124927.22336394</v>
       </c>
     </row>
     <row r="272">
@@ -3976,7 +3976,7 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>272657.33138657</v>
+        <v>124927.22336394</v>
       </c>
     </row>
     <row r="273">
@@ -3989,7 +3989,7 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>272667.28629998</v>
+        <v>124931.53671034</v>
       </c>
     </row>
     <row r="274">
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>272927.37293672</v>
+        <v>125041.11968798</v>
       </c>
     </row>
     <row r="275">
@@ -4015,7 +4015,7 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>272959.77496834</v>
+        <v>125055.77558577</v>
       </c>
     </row>
     <row r="276">
@@ -4028,7 +4028,7 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>273035.1979557</v>
+        <v>125088.37680808</v>
       </c>
     </row>
     <row r="277">
@@ -4041,7 +4041,7 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>273035.1979557</v>
+        <v>125088.37680808</v>
       </c>
     </row>
     <row r="278">
@@ -4054,7 +4054,7 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>273039.50749306</v>
+        <v>125090.31324916</v>
       </c>
     </row>
     <row r="279">
@@ -4067,7 +4067,7 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>273039.50749306</v>
+        <v>125090.31324916</v>
       </c>
     </row>
     <row r="280">
@@ -4080,7 +4080,7 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>273138.93061272</v>
+        <v>125134.70954348</v>
       </c>
     </row>
     <row r="281">
@@ -4093,7 +4093,7 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>273153.59198739</v>
+        <v>125141.19216682</v>
       </c>
     </row>
     <row r="282">
@@ -4106,7 +4106,7 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>273155.82801252</v>
+        <v>125142.19173708</v>
       </c>
     </row>
     <row r="283">
@@ -4119,7 +4119,7 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>273152.10252455</v>
+        <v>125140.50437506</v>
       </c>
     </row>
     <row r="284">
@@ -4132,7 +4132,7 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>273260.08832692</v>
+        <v>125189.3823319</v>
       </c>
     </row>
     <row r="285">
@@ -4145,7 +4145,7 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>273284.46722462</v>
+        <v>125198.31655446</v>
       </c>
     </row>
     <row r="286">
@@ -4158,7 +4158,7 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>273243.79261797</v>
+        <v>125179.7181336</v>
       </c>
     </row>
     <row r="287">
@@ -4171,7 +4171,7 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>273243.79261797</v>
+        <v>125179.7181336</v>
       </c>
     </row>
     <row r="288">
@@ -4184,7 +4184,7 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>273239.33457064</v>
+        <v>125177.72603196</v>
       </c>
     </row>
     <row r="289">
@@ -4197,7 +4197,7 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>273242.74667722</v>
+        <v>125179.25069799</v>
       </c>
     </row>
     <row r="290">
@@ -4210,7 +4210,7 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>273055.20325974</v>
+        <v>125092.72131696</v>
       </c>
     </row>
     <row r="291">
@@ -4223,7 +4223,7 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>273027.17784159</v>
+        <v>125080.29260493</v>
       </c>
     </row>
     <row r="292">
@@ -4236,7 +4236,7 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>272841.63191225</v>
+        <v>124997.38030809</v>
       </c>
     </row>
     <row r="293">
@@ -4249,7 +4249,7 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>272500.12492865</v>
+        <v>124844.70784338</v>
       </c>
     </row>
     <row r="294">
@@ -4262,7 +4262,7 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>272214.27521186</v>
+        <v>124724.39461811</v>
       </c>
     </row>
     <row r="295">
@@ -4275,7 +4275,7 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>272133.02169708</v>
+        <v>124690.03044382</v>
       </c>
     </row>
     <row r="296">
@@ -4288,7 +4288,7 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>272056.31781339</v>
+        <v>124657.59000282</v>
       </c>
     </row>
     <row r="297">
@@ -4301,7 +4301,7 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>271485.98444358</v>
+        <v>124418.20356032</v>
       </c>
     </row>
     <row r="298">
@@ -4314,7 +4314,7 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>271032.96761238</v>
+        <v>124227.60355634</v>
       </c>
     </row>
     <row r="299">
@@ -4327,7 +4327,7 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>270958.71665977</v>
+        <v>124196.17761418</v>
       </c>
     </row>
     <row r="300">
@@ -4340,7 +4340,7 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>270573.98530435</v>
+        <v>124034.1450489</v>
       </c>
     </row>
     <row r="301">
@@ -4353,7 +4353,7 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>269757.09722563</v>
+        <v>123691.6599318</v>
       </c>
     </row>
     <row r="302">
@@ -4366,7 +4366,7 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>269757.09722563</v>
+        <v>123691.6599318</v>
       </c>
     </row>
     <row r="303">
@@ -4379,7 +4379,7 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>269757.09722563</v>
+        <v>123691.6599318</v>
       </c>
     </row>
     <row r="304">
@@ -4392,7 +4392,7 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>269224.47966419</v>
+        <v>123468.15076206</v>
       </c>
     </row>
     <row r="305">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>268666.24399454</v>
+        <v>123232.8533199</v>
       </c>
     </row>
     <row r="306">
@@ -4418,7 +4418,7 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>266896.92001536</v>
+        <v>122487.16957234</v>
       </c>
     </row>
     <row r="307">
@@ -4431,7 +4431,7 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>262936.04888671</v>
+        <v>120814.33069119</v>
       </c>
     </row>
     <row r="308">
@@ -4444,7 +4444,7 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>261893.76769843</v>
+        <v>120382.91425095</v>
       </c>
     </row>
     <row r="309">
@@ -4457,7 +4457,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>260266.78474604</v>
+        <v>119693.61714513</v>
       </c>
     </row>
     <row r="310">
@@ -4470,7 +4470,7 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>258595.53304987</v>
+        <v>119002.9437661</v>
       </c>
     </row>
     <row r="311">
@@ -4483,7 +4483,7 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>254295.23375917</v>
+        <v>117235.68952503</v>
       </c>
     </row>
     <row r="312">
@@ -4496,7 +4496,7 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>251858.77468696</v>
+        <v>116238.18093334</v>
       </c>
     </row>
     <row r="313">
@@ -4509,7 +4509,7 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>251651.59360571</v>
+        <v>116148.11418568</v>
       </c>
     </row>
     <row r="314">
@@ -4522,7 +4522,7 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>250836.43575086</v>
+        <v>115799.16298925</v>
       </c>
     </row>
     <row r="315">
@@ -4535,7 +4535,7 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>250759.94714724</v>
+        <v>115766.19794197</v>
       </c>
     </row>
     <row r="316">
@@ -4548,7 +4548,7 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>250795.3575797</v>
+        <v>115782.22732114</v>
       </c>
     </row>
     <row r="317">
@@ -4561,7 +4561,7 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>250542.89149387</v>
+        <v>115671.82685922</v>
       </c>
     </row>
     <row r="318">
@@ -4574,7 +4574,7 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>250945.36508908</v>
+        <v>115839.6022011</v>
       </c>
     </row>
     <row r="319">
@@ -4587,7 +4587,7 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>250906.14947745</v>
+        <v>115823.21311319</v>
       </c>
     </row>
     <row r="320">
@@ -4600,7 +4600,7 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>250714.22319756</v>
+        <v>115739.03615569</v>
       </c>
     </row>
     <row r="321">
@@ -4613,7 +4613,7 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>250550.63752473</v>
+        <v>115667.63458987</v>
       </c>
     </row>
     <row r="322">
@@ -4626,7 +4626,7 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>252323.63502581</v>
+        <v>116534.38493613</v>
       </c>
     </row>
     <row r="323">
@@ -4639,7 +4639,7 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>252323.63502581</v>
+        <v>116534.38493613</v>
       </c>
     </row>
     <row r="324">
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>252269.10059932</v>
+        <v>116510.76247895</v>
       </c>
     </row>
     <row r="325">
@@ -4665,7 +4665,7 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>252173.8943786</v>
+        <v>116468.73374515</v>
       </c>
     </row>
     <row r="326">
@@ -4678,7 +4678,7 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>252189.51384332</v>
+        <v>116476.5396342</v>
       </c>
     </row>
     <row r="327">
@@ -4691,7 +4691,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>252084.84881408</v>
+        <v>116431.85835027</v>
       </c>
     </row>
     <row r="328">
@@ -4704,7 +4704,7 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>252730.06384654</v>
+        <v>116741.05660201</v>
       </c>
     </row>
     <row r="329">
@@ -4717,7 +4717,7 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>252554.81532758</v>
+        <v>116667.18320714</v>
       </c>
     </row>
     <row r="330">
@@ -4730,7 +4730,7 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>252554.81532758</v>
+        <v>116667.18320714</v>
       </c>
     </row>
     <row r="331">
@@ -4743,7 +4743,7 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>252386.21764648</v>
+        <v>116598.97545711</v>
       </c>
     </row>
     <row r="332">
@@ -4756,7 +4756,7 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>252420.56600986</v>
+        <v>116615.89100186</v>
       </c>
     </row>
     <row r="333">
@@ -4769,7 +4769,7 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>252226.63119585</v>
+        <v>116533.63734644</v>
       </c>
     </row>
     <row r="334">
@@ -4782,7 +4782,7 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>251770.52406069</v>
+        <v>116340.15991904</v>
       </c>
     </row>
     <row r="335">
@@ -4795,7 +4795,7 @@
         </is>
       </c>
       <c r="C335" t="n">
-        <v>251768.89035959</v>
+        <v>116337.99818145</v>
       </c>
     </row>
     <row r="336">
@@ -4808,7 +4808,7 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>251505.60890845</v>
+        <v>116227.07810773</v>
       </c>
     </row>
     <row r="337">
@@ -4821,7 +4821,7 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>251287.40635684</v>
+        <v>116133.63105732</v>
       </c>
     </row>
     <row r="338">
@@ -4834,7 +4834,7 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>251287.40635684</v>
+        <v>116133.63105732</v>
       </c>
     </row>
     <row r="339">
@@ -4847,7 +4847,7 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>250584.4982056</v>
+        <v>115831.73148276</v>
       </c>
     </row>
     <row r="340">
@@ -4860,7 +4860,7 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>250044.66489513</v>
+        <v>115601.92505959</v>
       </c>
     </row>
     <row r="341">
@@ -4873,7 +4873,7 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>250036.92965447</v>
+        <v>115598.59352755</v>
       </c>
     </row>
     <row r="342">
@@ -4886,7 +4886,7 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>249915.37837844</v>
+        <v>115546.21657178</v>
       </c>
     </row>
     <row r="343">
@@ -4899,7 +4899,7 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>249823.33818445</v>
+        <v>115506.57871061</v>
       </c>
     </row>
     <row r="344">
@@ -4912,7 +4912,7 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>249621.62880479</v>
+        <v>115420.44881361</v>
       </c>
     </row>
     <row r="345">
@@ -4925,7 +4925,7 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>249204.5563415</v>
+        <v>115235.81683435</v>
       </c>
     </row>
     <row r="346">
@@ -4938,7 +4938,7 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>249169.08878067</v>
+        <v>115219.51881977</v>
       </c>
     </row>
     <row r="347">
@@ -4951,7 +4951,7 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>249160.91596142</v>
+        <v>115215.77592972</v>
       </c>
     </row>
     <row r="348">
@@ -4964,7 +4964,7 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>248828.10739181</v>
+        <v>115071.85258577</v>
       </c>
     </row>
     <row r="349">
@@ -4977,7 +4977,7 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>248366.64952216</v>
+        <v>114875.88096072</v>
       </c>
     </row>
     <row r="350">
@@ -4990,7 +4990,7 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>247640.05700192</v>
+        <v>114546.14652338</v>
       </c>
     </row>
     <row r="351">
@@ -5003,7 +5003,7 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>247640.05700192</v>
+        <v>114546.14652338</v>
       </c>
     </row>
     <row r="352">
@@ -5016,7 +5016,7 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>247041.13150927</v>
+        <v>114281.24434674</v>
       </c>
     </row>
     <row r="353">
@@ -5029,7 +5029,7 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>246063.88431288</v>
+        <v>113831.48799207</v>
       </c>
     </row>
     <row r="354">
@@ -5042,7 +5042,7 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>246063.88431288</v>
+        <v>113831.48799207</v>
       </c>
     </row>
     <row r="355">
@@ -5055,7 +5055,7 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>245870.95250086</v>
+        <v>113742.34262015</v>
       </c>
     </row>
     <row r="356">
@@ -5068,7 +5068,7 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>245447.3751357</v>
+        <v>113560.79259307</v>
       </c>
     </row>
     <row r="357">
@@ -5081,7 +5081,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>245055.49077255</v>
+        <v>113379.36898293</v>
       </c>
     </row>
     <row r="358">
@@ -5094,7 +5094,7 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>245055.49077255</v>
+        <v>113379.36898293</v>
       </c>
     </row>
     <row r="359">
@@ -5107,7 +5107,7 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>244281.89783946</v>
+        <v>113040.51874646</v>
       </c>
     </row>
     <row r="360">
@@ -5120,7 +5120,7 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>244337.77598544</v>
+        <v>113069.5805629</v>
       </c>
     </row>
     <row r="361">
@@ -5133,7 +5133,7 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>244337.77598544</v>
+        <v>113069.5805629</v>
       </c>
     </row>
     <row r="362">
@@ -5146,7 +5146,7 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>244340.64280969</v>
+        <v>113070.86179032</v>
       </c>
     </row>
     <row r="363">
@@ -5159,7 +5159,7 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>244461.7117475</v>
+        <v>113130.54043847</v>
       </c>
     </row>
     <row r="364">
@@ -5172,7 +5172,7 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>244434.47805482</v>
+        <v>113117.95325513</v>
       </c>
     </row>
     <row r="365">
@@ -5185,7 +5185,7 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>244502.43842026</v>
+        <v>113148.50540621</v>
       </c>
     </row>
     <row r="366">
@@ -5198,7 +5198,7 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>244502.43842026</v>
+        <v>113148.50540621</v>
       </c>
     </row>
     <row r="367">
@@ -5211,7 +5211,7 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>244215.87850602</v>
+        <v>113027.68732558</v>
       </c>
     </row>
     <row r="368">
@@ -5224,7 +5224,7 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>244203.76297665</v>
+        <v>113022.18652121</v>
       </c>
     </row>
     <row r="369">
@@ -5237,7 +5237,7 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>244071.63481639</v>
+        <v>112966.86516115</v>
       </c>
     </row>
     <row r="370">
@@ -5250,7 +5250,7 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>244181.68430148</v>
+        <v>113015.91748001</v>
       </c>
     </row>
     <row r="371">
@@ -5263,7 +5263,7 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>244168.540719</v>
+        <v>113011.25893998</v>
       </c>
     </row>
     <row r="372">
@@ -5276,7 +5276,7 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>244503.88774417</v>
+        <v>113153.95717747</v>
       </c>
     </row>
     <row r="373">
@@ -5289,7 +5289,7 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>244468.12086061</v>
+        <v>113137.26638155</v>
       </c>
     </row>
     <row r="374">
@@ -5302,7 +5302,7 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>244467.00308397</v>
+        <v>113136.78168573</v>
       </c>
     </row>
     <row r="375">
@@ -5315,7 +5315,7 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>244481.50909986</v>
+        <v>113143.15598394</v>
       </c>
     </row>
     <row r="376">
@@ -5328,7 +5328,7 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>244715.18160203</v>
+        <v>113246.04543436</v>
       </c>
     </row>
     <row r="377">
@@ -5341,7 +5341,7 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>244848.68116537</v>
+        <v>113304.44798242</v>
       </c>
     </row>
     <row r="378">
@@ -5354,7 +5354,7 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>244948.74448656</v>
+        <v>113346.81620964</v>
       </c>
     </row>
     <row r="379">
@@ -5367,7 +5367,7 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>244908.59845749</v>
+        <v>113329.49598246</v>
       </c>
     </row>
     <row r="380">
@@ -5380,7 +5380,7 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>244618.35500287</v>
+        <v>113205.7372292</v>
       </c>
     </row>
     <row r="381">
@@ -5393,7 +5393,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>244644.56075683</v>
+        <v>113216.82868722</v>
       </c>
     </row>
     <row r="382">
@@ -5406,7 +5406,7 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>244719.03795172</v>
+        <v>113248.85630082</v>
       </c>
     </row>
     <row r="383">
@@ -5419,7 +5419,7 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>244651.59611178</v>
+        <v>113220.25491014</v>
       </c>
     </row>
     <row r="384">
@@ -5432,7 +5432,7 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>244647.85214297</v>
+        <v>113218.69182342</v>
       </c>
     </row>
     <row r="385">
@@ -5445,7 +5445,7 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>244654.14558553</v>
+        <v>113221.50162936</v>
       </c>
     </row>
     <row r="386">
@@ -5458,7 +5458,7 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>244589.02273087</v>
+        <v>113193.74381843</v>
       </c>
     </row>
     <row r="387">
@@ -5471,7 +5471,7 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>244631.837204</v>
+        <v>113212.98089333</v>
       </c>
     </row>
     <row r="388">
@@ -5484,7 +5484,7 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>244773.12005986</v>
+        <v>113274.26038529</v>
       </c>
     </row>
     <row r="389">
@@ -5497,7 +5497,7 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>244773.12005986</v>
+        <v>113274.26038529</v>
       </c>
     </row>
     <row r="390">
@@ -5510,7 +5510,7 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>244759.72342403</v>
+        <v>113268.52434887</v>
       </c>
     </row>
     <row r="391">
@@ -5523,7 +5523,7 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>244759.72342403</v>
+        <v>113268.52434887</v>
       </c>
     </row>
     <row r="392">
@@ -5536,7 +5536,7 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>244748.27656503</v>
+        <v>113263.10121803</v>
       </c>
     </row>
     <row r="393">
@@ -5549,7 +5549,7 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>244741.17804762</v>
+        <v>113259.98563409</v>
       </c>
     </row>
     <row r="394">
@@ -5562,7 +5562,7 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>244744.6333423</v>
+        <v>113261.49662022</v>
       </c>
     </row>
     <row r="395">
@@ -5575,7 +5575,7 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>244794.61502008</v>
+        <v>113283.04453747</v>
       </c>
     </row>
     <row r="396">
@@ -5588,7 +5588,7 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>244756.54113378</v>
+        <v>113265.40012513</v>
       </c>
     </row>
     <row r="397">
@@ -5601,7 +5601,7 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>244431.28320931</v>
+        <v>113114.10550717</v>
       </c>
     </row>
     <row r="398">
@@ -5614,7 +5614,7 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>244309.72149425</v>
+        <v>113057.31587493</v>
       </c>
     </row>
     <row r="399">
@@ -5627,7 +5627,7 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>244000.73032356</v>
+        <v>112914.15136645</v>
       </c>
     </row>
     <row r="400">
@@ -5640,7 +5640,7 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>243144.15724525</v>
+        <v>112514.4442759</v>
       </c>
     </row>
     <row r="401">
@@ -5653,7 +5653,7 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>243024.12950515</v>
+        <v>112458.52835665</v>
       </c>
     </row>
     <row r="402">
@@ -5666,7 +5666,7 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>241858.01687663</v>
+        <v>111915.73673453</v>
       </c>
     </row>
     <row r="403">
@@ -5679,7 +5679,7 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>240711.02800084</v>
+        <v>111381.25397377</v>
       </c>
     </row>
     <row r="404">
@@ -5692,7 +5692,7 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>240132.61683964</v>
+        <v>111111.51666858</v>
       </c>
     </row>
     <row r="405">
@@ -5705,7 +5705,7 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>236882.15953231</v>
+        <v>109592.41819814</v>
       </c>
     </row>
     <row r="406">
@@ -5718,7 +5718,7 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>236131.60209258</v>
+        <v>109239.32247663</v>
       </c>
     </row>
     <row r="407">
@@ -5731,7 +5731,7 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>234979.15327233</v>
+        <v>108698.33847377</v>
       </c>
     </row>
     <row r="408">
@@ -5744,7 +5744,7 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>234989.03574465</v>
+        <v>108702.95001848</v>
       </c>
     </row>
     <row r="409">
@@ -5757,7 +5757,7 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>234976.19600066</v>
+        <v>108697.78900613</v>
       </c>
     </row>
     <row r="410">
@@ -5770,7 +5770,7 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>234918.54772319</v>
+        <v>108673.29704941</v>
       </c>
     </row>
     <row r="411">
@@ -5783,7 +5783,7 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>234918.54772319</v>
+        <v>108673.29704941</v>
       </c>
     </row>
     <row r="412">
@@ -5796,7 +5796,7 @@
         </is>
       </c>
       <c r="C412" t="n">
-        <v>234938.83859561</v>
+        <v>108682.44353315</v>
       </c>
     </row>
     <row r="413">
@@ -5809,7 +5809,7 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>234939.20422424</v>
+        <v>108682.87489085</v>
       </c>
     </row>
     <row r="414">
@@ -5822,7 +5822,7 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>234934.96239986</v>
+        <v>108680.98093892</v>
       </c>
     </row>
     <row r="415">
@@ -5835,7 +5835,7 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>234923.94228705</v>
+        <v>108676.33157682</v>
       </c>
     </row>
     <row r="416">
@@ -5848,7 +5848,7 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>234929.48264432</v>
+        <v>108678.77746759</v>
       </c>
     </row>
     <row r="417">
@@ -5861,7 +5861,7 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>234948.87522894</v>
+        <v>108686.86716162</v>
       </c>
     </row>
     <row r="418">
@@ -5874,7 +5874,7 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>234445.48195319</v>
+        <v>108448.15878296</v>
       </c>
     </row>
     <row r="419">
@@ -5887,7 +5887,7 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>234457.17311688</v>
+        <v>108453.44290499</v>
       </c>
     </row>
     <row r="420">
@@ -5900,7 +5900,7 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>234630.36158873</v>
+        <v>108534.57836023</v>
       </c>
     </row>
     <row r="421">
@@ -5913,7 +5913,7 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>234630.36158873</v>
+        <v>108534.57836023</v>
       </c>
     </row>
     <row r="422">
@@ -5926,7 +5926,7 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>234636.4698798</v>
+        <v>108537.27909687</v>
       </c>
     </row>
     <row r="423">
@@ -5939,7 +5939,7 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>234656.72955716</v>
+        <v>108546.18740486</v>
       </c>
     </row>
     <row r="424">
@@ -5952,7 +5952,7 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>234684.22328905</v>
+        <v>108558.18503729</v>
       </c>
     </row>
     <row r="425">
@@ -5965,7 +5965,7 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>234689.55221368</v>
+        <v>108560.55165108</v>
       </c>
     </row>
     <row r="426">
@@ -5978,7 +5978,7 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>234602.34123491</v>
+        <v>108523.41650927</v>
       </c>
     </row>
     <row r="427">
@@ -5991,7 +5991,7 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>234620.34864603</v>
+        <v>108531.79452511</v>
       </c>
     </row>
     <row r="428">
@@ -6004,7 +6004,7 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>234760.56948558</v>
+        <v>108591.67695408</v>
       </c>
     </row>
     <row r="429">
@@ -6017,7 +6017,7 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>234762.47899519</v>
+        <v>108592.57730295</v>
       </c>
     </row>
     <row r="430">
@@ -6030,7 +6030,7 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>234760.95445938</v>
+        <v>108591.89301205</v>
       </c>
     </row>
     <row r="431">
@@ -6043,7 +6043,7 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>234817.27712572</v>
+        <v>108617.38159267</v>
       </c>
     </row>
     <row r="432">
@@ -6056,7 +6056,7 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>234835.02561726</v>
+        <v>108625.08741793</v>
       </c>
     </row>
     <row r="433">
@@ -6069,7 +6069,7 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>234838.88777758</v>
+        <v>108626.80586908</v>
       </c>
     </row>
     <row r="434">
@@ -6082,7 +6082,7 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>234843.85988964</v>
+        <v>108628.9026975</v>
       </c>
     </row>
     <row r="435">
@@ -6095,7 +6095,7 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>234848.47018835</v>
+        <v>108630.89151317</v>
       </c>
     </row>
     <row r="436">
@@ -6108,7 +6108,7 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>234843.90161134</v>
+        <v>108629.47034503</v>
       </c>
     </row>
     <row r="437">
@@ -6121,7 +6121,7 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>234816.96616625</v>
+        <v>108617.28558268</v>
       </c>
     </row>
     <row r="438">
@@ -6134,7 +6134,7 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>234939.5970838</v>
+        <v>108669.38740316</v>
       </c>
     </row>
     <row r="439">
@@ -6147,7 +6147,7 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>234965.30354115</v>
+        <v>108680.19081614</v>
       </c>
     </row>
     <row r="440">
@@ -6160,7 +6160,7 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>234968.2156281</v>
+        <v>108681.49564846</v>
       </c>
     </row>
     <row r="441">
@@ -6173,7 +6173,7 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>234970.7394673</v>
+        <v>108682.59912121</v>
       </c>
     </row>
     <row r="442">
@@ -6186,7 +6186,7 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>234971.60206947</v>
+        <v>108682.97895581</v>
       </c>
     </row>
     <row r="443">
@@ -6199,7 +6199,7 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>234973.06338791</v>
+        <v>108683.6307655</v>
       </c>
     </row>
     <row r="444">
@@ -6212,7 +6212,7 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>234975.22901823</v>
+        <v>108684.57459476</v>
       </c>
     </row>
     <row r="445">
@@ -6225,7 +6225,7 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>234975.22901823</v>
+        <v>108684.57459476</v>
       </c>
     </row>
     <row r="446">
@@ -6238,7 +6238,7 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>234977.83956085</v>
+        <v>108685.71145137</v>
       </c>
     </row>
     <row r="447">
@@ -6251,7 +6251,7 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>234987.33032808</v>
+        <v>108689.92527425</v>
       </c>
     </row>
     <row r="448">
@@ -6264,7 +6264,7 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>235016.00272113</v>
+        <v>108702.28238008</v>
       </c>
     </row>
     <row r="449">
@@ -6277,7 +6277,7 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>235016.56121766</v>
+        <v>108702.52751655</v>
       </c>
     </row>
     <row r="450">
@@ -6290,7 +6290,7 @@
         </is>
       </c>
       <c r="C450" t="n">
-        <v>235042.80979372</v>
+        <v>108713.96073111</v>
       </c>
     </row>
     <row r="451">
@@ -6303,7 +6303,7 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>235061.55950167</v>
+        <v>108722.30114313</v>
       </c>
     </row>
     <row r="452">
@@ -6316,7 +6316,7 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>235061.55950167</v>
+        <v>108722.30114313</v>
       </c>
     </row>
     <row r="453">
@@ -6329,7 +6329,7 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>235065.05643446</v>
+        <v>108723.82967512</v>
       </c>
     </row>
     <row r="454">
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>235063.66910312</v>
+        <v>108723.2920416</v>
       </c>
     </row>
     <row r="455">
@@ -6355,7 +6355,7 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>235063.66910312</v>
+        <v>108723.2920416</v>
       </c>
     </row>
     <row r="456">
@@ -6368,7 +6368,7 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>235053.92923528</v>
+        <v>108718.40691596</v>
       </c>
     </row>
     <row r="457">
@@ -6381,7 +6381,7 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>235062.5089055</v>
+        <v>108722.04137561</v>
       </c>
     </row>
     <row r="458">
@@ -6394,7 +6394,7 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>235068.09640551</v>
+        <v>108724.49470255</v>
       </c>
     </row>
     <row r="459">
@@ -6407,7 +6407,7 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>235066.7600546</v>
+        <v>108723.94825406</v>
       </c>
     </row>
     <row r="460">
@@ -6420,7 +6420,7 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>235126.33185526</v>
+        <v>108749.03488553</v>
       </c>
     </row>
     <row r="461">
@@ -6433,7 +6433,7 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>235126.57730159</v>
+        <v>108749.14226977</v>
       </c>
     </row>
     <row r="462">
@@ -6446,7 +6446,7 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>235142.77086953</v>
+        <v>108755.88937851</v>
       </c>
     </row>
     <row r="463">
@@ -6459,7 +6459,7 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>235176.89272764</v>
+        <v>108770.57313768</v>
       </c>
     </row>
     <row r="464">
@@ -6472,7 +6472,7 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>235158.40756019</v>
+        <v>108762.64541579</v>
       </c>
     </row>
     <row r="465">
@@ -6485,7 +6485,7 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>235180.14159182</v>
+        <v>108772.49453963</v>
       </c>
     </row>
     <row r="466">
@@ -6498,7 +6498,7 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>235200.18228615</v>
+        <v>108781.24495701</v>
       </c>
     </row>
     <row r="467">
@@ -6511,7 +6511,7 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>235220.43874574</v>
+        <v>108790.08490544</v>
       </c>
     </row>
     <row r="468">
@@ -6524,7 +6524,7 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>235219.69491343</v>
+        <v>108789.76048755</v>
       </c>
     </row>
     <row r="469">
@@ -6537,7 +6537,7 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>235208.39242183</v>
+        <v>108784.91554714</v>
       </c>
     </row>
     <row r="470">
@@ -6550,7 +6550,7 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>235208.39242183</v>
+        <v>108784.91554714</v>
       </c>
     </row>
     <row r="471">
@@ -6563,7 +6563,7 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>235208.39242183</v>
+        <v>108784.91554714</v>
       </c>
     </row>
     <row r="472">
@@ -6576,7 +6576,7 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>235209.25114082</v>
+        <v>108785.2915559</v>
       </c>
     </row>
     <row r="473">
@@ -6589,7 +6589,7 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>235317.48354275</v>
+        <v>108833.27472732</v>
       </c>
     </row>
     <row r="474">
@@ -6602,7 +6602,7 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>235318.51053574</v>
+        <v>108833.72079142</v>
       </c>
     </row>
     <row r="475">
@@ -6615,7 +6615,7 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>235325.54615264</v>
+        <v>108836.78986723</v>
       </c>
     </row>
     <row r="476">
@@ -6628,7 +6628,7 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>235325.83569318</v>
+        <v>108836.9175853</v>
       </c>
     </row>
     <row r="477">
@@ -6641,7 +6641,7 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>235423.70719258</v>
+        <v>108881.40199022</v>
       </c>
     </row>
     <row r="478">
@@ -6654,7 +6654,7 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>235382.18774824</v>
+        <v>108862.50139058</v>
       </c>
     </row>
     <row r="479">
@@ -6667,7 +6667,7 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>235382.18774824</v>
+        <v>108862.50139058</v>
       </c>
     </row>
     <row r="480">
@@ -6680,7 +6680,7 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>235397.83797772</v>
+        <v>108869.43422765</v>
       </c>
     </row>
     <row r="481">
@@ -6693,7 +6693,7 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>235401.26838163</v>
+        <v>108870.96988734</v>
       </c>
     </row>
     <row r="482">
@@ -6706,7 +6706,7 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>235411.42959141</v>
+        <v>108875.43642171</v>
       </c>
     </row>
     <row r="483">
@@ -6719,7 +6719,7 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>235428.75484962</v>
+        <v>108883.07930522</v>
       </c>
     </row>
     <row r="484">
@@ -6732,7 +6732,7 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>235464.21031155</v>
+        <v>108898.38025272</v>
       </c>
     </row>
     <row r="485">
@@ -6745,7 +6745,7 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>235470.39635743</v>
+        <v>108901.0704302</v>
       </c>
     </row>
     <row r="486">
@@ -6758,7 +6758,7 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>235469.60070089</v>
+        <v>108900.68172438</v>
       </c>
     </row>
     <row r="487">
@@ -6771,7 +6771,7 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>235469.60070089</v>
+        <v>108900.68172438</v>
       </c>
     </row>
     <row r="488">
@@ -6784,7 +6784,7 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>235474.1687663</v>
+        <v>108902.72156459</v>
       </c>
     </row>
     <row r="489">
@@ -6797,7 +6797,7 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>235481.53595641</v>
+        <v>108905.88759933</v>
       </c>
     </row>
     <row r="490">
@@ -6810,7 +6810,7 @@
         </is>
       </c>
       <c r="C490" t="n">
-        <v>235508.89054277</v>
+        <v>108918.24424234</v>
       </c>
     </row>
     <row r="491">
@@ -6823,7 +6823,7 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>235508.89054277</v>
+        <v>108918.24424234</v>
       </c>
     </row>
     <row r="492">
@@ -6836,7 +6836,7 @@
         </is>
       </c>
       <c r="C492" t="n">
-        <v>235521.54327529</v>
+        <v>108923.87408837</v>
       </c>
     </row>
     <row r="493">
@@ -6849,7 +6849,7 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>235537.21541127</v>
+        <v>108930.74111592</v>
       </c>
     </row>
     <row r="494">
@@ -6862,7 +6862,7 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>235564.92806286</v>
+        <v>108943.0469027</v>
       </c>
     </row>
     <row r="495">
@@ -6875,7 +6875,7 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>235564.9319284</v>
+        <v>108943.07138778</v>
       </c>
     </row>
     <row r="496">
@@ -6888,7 +6888,7 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>235570.02564257</v>
+        <v>108945.26065161</v>
       </c>
     </row>
     <row r="497">
@@ -6901,7 +6901,7 @@
         </is>
       </c>
       <c r="C497" t="n">
-        <v>235588.33157316</v>
+        <v>108953.15641341</v>
       </c>
     </row>
     <row r="498">
@@ -6914,7 +6914,7 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>235624.36244039</v>
+        <v>108968.57761536</v>
       </c>
     </row>
     <row r="499">
@@ -6927,7 +6927,7 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>235640.02210373</v>
+        <v>108975.38776857</v>
       </c>
     </row>
     <row r="500">
@@ -6940,7 +6940,7 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>235646.87939131</v>
+        <v>108978.42741255</v>
       </c>
     </row>
     <row r="501">
@@ -6953,7 +6953,7 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>235648.07792634</v>
+        <v>108978.95279825</v>
       </c>
     </row>
     <row r="502">
@@ -6966,7 +6966,7 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>235648.40369046</v>
+        <v>108979.09543129</v>
       </c>
     </row>
     <row r="503">
@@ -6979,7 +6979,7 @@
         </is>
       </c>
       <c r="C503" t="n">
-        <v>235658.09755057</v>
+        <v>108983.32012715</v>
       </c>
     </row>
     <row r="504">
@@ -6992,7 +6992,7 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>235716.97638491</v>
+        <v>109008.73801967</v>
       </c>
     </row>
     <row r="505">
@@ -7005,7 +7005,7 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>235747.28391856</v>
+        <v>109022.02499029</v>
       </c>
     </row>
     <row r="506">
@@ -7018,7 +7018,7 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>235756.19903116</v>
+        <v>109025.88959254</v>
       </c>
     </row>
     <row r="507">
@@ -7031,7 +7031,7 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>235753.18291993</v>
+        <v>109024.59805526</v>
       </c>
     </row>
     <row r="508">
@@ -7044,7 +7044,7 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>235759.38016474</v>
+        <v>109027.29709849</v>
       </c>
     </row>
     <row r="509">
@@ -7057,7 +7057,7 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>235760.67345533</v>
+        <v>109027.87908413</v>
       </c>
     </row>
     <row r="510">
@@ -7070,7 +7070,7 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>235770.31293069</v>
+        <v>109031.94039429</v>
       </c>
     </row>
     <row r="511">
@@ -7083,7 +7083,7 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>235778.77709791</v>
+        <v>109035.79046511</v>
       </c>
     </row>
     <row r="512">
@@ -7096,7 +7096,7 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>235809.23853334</v>
+        <v>109048.93534851</v>
       </c>
     </row>
     <row r="513">
@@ -7109,7 +7109,7 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>235851.97722934</v>
+        <v>109067.82129496</v>
       </c>
     </row>
     <row r="514">
@@ -7122,7 +7122,7 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>235889.86419984</v>
+        <v>109084.87642944</v>
       </c>
     </row>
     <row r="515">
@@ -7135,7 +7135,7 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>235917.7875033</v>
+        <v>109097.08051312</v>
       </c>
     </row>
     <row r="516">
@@ -7148,7 +7148,7 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>235917.52259809</v>
+        <v>109096.96209519</v>
       </c>
     </row>
     <row r="517">
@@ -7161,7 +7161,7 @@
         </is>
       </c>
       <c r="C517" t="n">
-        <v>235928.04665396</v>
+        <v>109101.48523202</v>
       </c>
     </row>
     <row r="518">
@@ -7174,7 +7174,7 @@
         </is>
       </c>
       <c r="C518" t="n">
-        <v>235940.9540861</v>
+        <v>109107.21215637</v>
       </c>
     </row>
     <row r="519">
@@ -7187,7 +7187,7 @@
         </is>
       </c>
       <c r="C519" t="n">
-        <v>235948.54070558</v>
+        <v>109110.67118091</v>
       </c>
     </row>
     <row r="520">
@@ -7200,7 +7200,7 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>235945.16586083</v>
+        <v>109109.20219063</v>
       </c>
     </row>
     <row r="521">
@@ -7213,7 +7213,7 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>235945.86705687</v>
+        <v>109109.51175791</v>
       </c>
     </row>
     <row r="522">
@@ -7226,7 +7226,7 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>235946.29645468</v>
+        <v>109109.69944321</v>
       </c>
     </row>
     <row r="523">
@@ -7239,7 +7239,7 @@
         </is>
       </c>
       <c r="C523" t="n">
-        <v>235952.90318939</v>
+        <v>109112.58601586</v>
       </c>
     </row>
     <row r="524">
@@ -7252,7 +7252,7 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>235969.65351988</v>
+        <v>109119.9922244</v>
       </c>
     </row>
     <row r="525">
@@ -7265,7 +7265,7 @@
         </is>
       </c>
       <c r="C525" t="n">
-        <v>235986.02125875</v>
+        <v>109127.24998387</v>
       </c>
     </row>
     <row r="526">
@@ -7278,7 +7278,7 @@
         </is>
       </c>
       <c r="C526" t="n">
-        <v>235980.19175737</v>
+        <v>109124.69313171</v>
       </c>
     </row>
     <row r="527">
@@ -7291,7 +7291,7 @@
         </is>
       </c>
       <c r="C527" t="n">
-        <v>235992.35996945</v>
+        <v>109130.13976517</v>
       </c>
     </row>
     <row r="528">
@@ -7304,7 +7304,7 @@
         </is>
       </c>
       <c r="C528" t="n">
-        <v>236015.1053727</v>
+        <v>109140.11003654</v>
       </c>
     </row>
     <row r="529">
@@ -7317,7 +7317,7 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>236021.62210069</v>
+        <v>109142.96072876</v>
       </c>
     </row>
     <row r="530">
@@ -7330,7 +7330,7 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>236021.3975028</v>
+        <v>109142.86240892</v>
       </c>
     </row>
     <row r="531">
@@ -7343,7 +7343,215 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>236026.60844911</v>
+        <v>109145.10674065</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="2" t="n">
+        <v>44988.00577546296</v>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>1677798499</t>
+        </is>
+      </c>
+      <c r="C532" t="n">
+        <v>109144.22581393</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="2" t="n">
+        <v>44988.01210648148</v>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>1677799046</t>
+        </is>
+      </c>
+      <c r="C533" t="n">
+        <v>109144.22581393</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="2" t="n">
+        <v>44989.03908564815</v>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>1677887777</t>
+        </is>
+      </c>
+      <c r="C534" t="n">
+        <v>109144.86160044</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="2" t="n">
+        <v>44990.02949074074</v>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>1677973348</t>
+        </is>
+      </c>
+      <c r="C535" t="n">
+        <v>109145.94831197</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="2" t="n">
+        <v>44991.01837962963</v>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>1678058788</t>
+        </is>
+      </c>
+      <c r="C536" t="n">
+        <v>109147.3061139</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="2" t="n">
+        <v>44992.1540625</v>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>1678156911</t>
+        </is>
+      </c>
+      <c r="C537" t="n">
+        <v>109157.97074703</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="2" t="n">
+        <v>44993.03241898148</v>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>1678232801</t>
+        </is>
+      </c>
+      <c r="C538" t="n">
+        <v>109166.9156174</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="2" t="n">
+        <v>44994.02148148148</v>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>1678318256</t>
+        </is>
+      </c>
+      <c r="C539" t="n">
+        <v>109166.9156174</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="2" t="n">
+        <v>44995.39335648148</v>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>1678436786</t>
+        </is>
+      </c>
+      <c r="C540" t="n">
+        <v>109172.68510872</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="2" t="n">
+        <v>44995.96583333334</v>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>1678486248</t>
+        </is>
+      </c>
+      <c r="C541" t="n">
+        <v>109174.59736808</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="2" t="n">
+        <v>44997.02534722222</v>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>1678577790</t>
+        </is>
+      </c>
+      <c r="C542" t="n">
+        <v>109179.43015703</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="2" t="n">
+        <v>44998.01040509259</v>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>1678662899</t>
+        </is>
+      </c>
+      <c r="C543" t="n">
+        <v>109191.91109749</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="2" t="n">
+        <v>44999.03914351852</v>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>1678751782</t>
+        </is>
+      </c>
+      <c r="C544" t="n">
+        <v>109191.54982029</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="2" t="n">
+        <v>44999.971875</v>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>1678832370</t>
+        </is>
+      </c>
+      <c r="C545" t="n">
+        <v>109193.85578451</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="2" t="n">
+        <v>45001.04237268519</v>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>1678924861</t>
+        </is>
+      </c>
+      <c r="C546" t="n">
+        <v>109194.38292894</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="2" t="n">
+        <v>45001.08371527777</v>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>1678928433</t>
+        </is>
+      </c>
+      <c r="C547" t="n">
+        <v>109194.33406936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>